<commit_message>
first completed version of optim app
</commit_message>
<xml_diff>
--- a/data/OPZ.xlsx
+++ b/data/OPZ.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="48">
   <si>
     <t>supply_road</t>
   </si>
@@ -58,6 +58,9 @@
     <t>ГОР</t>
   </si>
   <si>
+    <t>ДВС</t>
+  </si>
+  <si>
     <t>ДОН</t>
   </si>
   <si>
@@ -70,12 +73,15 @@
     <t>КЗХ</t>
   </si>
   <si>
-    <t>ЛАТ</t>
+    <t>КЛГ</t>
   </si>
   <si>
     <t>МСК</t>
   </si>
   <si>
+    <t>ОДС</t>
+  </si>
+  <si>
     <t>ОКТ</t>
   </si>
   <si>
@@ -106,34 +112,52 @@
     <t>Под погрузку в 8 сутки</t>
   </si>
   <si>
-    <t>В промывку на дорогу: ВСБ</t>
+    <t>Под погрузку в 10 сутки</t>
+  </si>
+  <si>
+    <t>Из под НПГ без промывки под аналогичный груз КБШ</t>
+  </si>
+  <si>
+    <t>Под погрузку в 15 сутки</t>
+  </si>
+  <si>
+    <t>Сдвоенная операция ГОР</t>
+  </si>
+  <si>
+    <t>В промывку на дорогу: ГОР</t>
+  </si>
+  <si>
+    <t>Из под НПГ без промывки под аналогичный груз ГОР</t>
+  </si>
+  <si>
+    <t>В кольце на дорогу: ГОР</t>
+  </si>
+  <si>
+    <t>Затягивание грузовой операции на дороге: ДВС</t>
   </si>
   <si>
     <t>Под погрузку в 5 сутки</t>
   </si>
   <si>
-    <t>В аренду на дорогу: ЮВС</t>
-  </si>
-  <si>
-    <t>Затягивание грузовой операции на дороге: КЗХ</t>
-  </si>
-  <si>
-    <t>Затягивание грузовой операции на дороге: ЛАТ</t>
-  </si>
-  <si>
-    <t>В промывку на дорогу: ОКТ</t>
-  </si>
-  <si>
-    <t>В ремонт на дорогу: ПРВ</t>
-  </si>
-  <si>
-    <t>В отстой на дорогу: СКВ</t>
-  </si>
-  <si>
-    <t>В кольце на дорогу: УЗБ</t>
-  </si>
-  <si>
-    <t>В промывку на дорогу: УЗБ</t>
+    <t>В кольце на дорогу: ЗСБ</t>
+  </si>
+  <si>
+    <t>В ремонт на дорогу: ЗСБ</t>
+  </si>
+  <si>
+    <t>В распыление на дорогу: ЮВС</t>
+  </si>
+  <si>
+    <t>В ремонт на дорогу: КБШ</t>
+  </si>
+  <si>
+    <t>Из под НПГ без промывки под аналогичный груз ОДС</t>
+  </si>
+  <si>
+    <t>Из под НПГ без промывки под аналогичный груз ОКТ</t>
+  </si>
+  <si>
+    <t>В ремонт на дорогу: СКВ</t>
   </si>
 </sst>
 </file>
@@ -494,7 +518,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J29"/>
+  <dimension ref="A1:J53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -559,13 +583,13 @@
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="I2" s="1">
         <v>31</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="20" customHeight="1">
@@ -591,13 +615,13 @@
         <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="I3" s="1">
         <v>42</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="20" customHeight="1">
@@ -623,206 +647,122 @@
         <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>12</v>
+        <v>29</v>
       </c>
       <c r="I4" s="1">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="20" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="1">
+      <c r="H5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="1">
+        <v>2</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="20" customHeight="1">
+      <c r="H6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="1">
-        <v>222</v>
-      </c>
-      <c r="D5" s="1">
-        <v>128</v>
-      </c>
-      <c r="E5" s="1">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="I6" s="1">
         <v>4</v>
       </c>
-      <c r="G5" s="1">
-        <v>0</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="1">
-        <v>28</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="20" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1">
-        <v>11</v>
-      </c>
-      <c r="C6" s="1">
-        <v>14</v>
-      </c>
-      <c r="D6" s="1">
-        <v>0</v>
-      </c>
-      <c r="E6" s="1">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I6" s="1">
-        <v>11</v>
-      </c>
       <c r="J6" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="20" customHeight="1">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="C7" s="1">
-        <v>95</v>
+        <v>222</v>
       </c>
       <c r="D7" s="1">
-        <v>0</v>
+        <v>128</v>
       </c>
       <c r="E7" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F7" s="1">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="G7" s="1">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I7" s="1">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="20" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="1">
-        <v>41</v>
-      </c>
-      <c r="C8" s="1">
-        <v>74</v>
-      </c>
-      <c r="D8" s="1">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>31</v>
-      </c>
       <c r="H8" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I8" s="1">
-        <v>41</v>
+        <v>1</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="20" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="1">
-        <v>20</v>
-      </c>
-      <c r="C9" s="1">
-        <v>80</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
       <c r="H9" s="1" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="I9" s="1">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="20" customHeight="1">
       <c r="H10" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="I10" s="1">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="20" customHeight="1">
       <c r="H11" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="I11" s="1">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:10" ht="20" customHeight="1">
       <c r="A12" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B12" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C12" s="1">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="D12" s="1">
         <v>0</v>
@@ -837,152 +777,110 @@
         <v>0</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I12" s="1">
-        <v>43</v>
+        <v>2</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>34</v>
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="20" customHeight="1">
       <c r="A13" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B13" s="1">
-        <v>79</v>
+        <v>11</v>
       </c>
       <c r="C13" s="1">
-        <v>240</v>
+        <v>14</v>
       </c>
       <c r="D13" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="E13" s="1">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="F13" s="1">
-        <v>88</v>
+        <v>0</v>
       </c>
       <c r="G13" s="1">
-        <v>173</v>
+        <v>0</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="I13" s="1">
-        <v>79</v>
+        <v>11</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="20" customHeight="1">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B14" s="1">
-        <v>72</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1">
-        <v>200</v>
+        <v>95</v>
       </c>
       <c r="D14" s="1">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="E14" s="1">
-        <v>180</v>
+        <v>0</v>
       </c>
       <c r="F14" s="1">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="G14" s="1">
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="I14" s="1">
-        <v>100</v>
+        <v>11</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="20" customHeight="1">
-      <c r="A15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="1">
-        <v>5</v>
-      </c>
-      <c r="C15" s="1">
-        <v>428</v>
-      </c>
-      <c r="D15" s="1">
+      <c r="H15" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I15" s="1">
+        <v>14</v>
+      </c>
+      <c r="J15" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="E15" s="1">
-        <v>47</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
-        <v>124</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I15" s="1">
-        <v>5</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>36</v>
-      </c>
     </row>
     <row r="16" spans="1:10" ht="20" customHeight="1">
-      <c r="A16" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="1">
-        <v>19</v>
-      </c>
-      <c r="C16" s="1">
-        <v>125</v>
-      </c>
-      <c r="D16" s="1">
-        <v>0</v>
-      </c>
-      <c r="E16" s="1">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <v>10</v>
-      </c>
-      <c r="G16" s="1">
-        <v>35</v>
-      </c>
       <c r="H16" s="1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="I16" s="1">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="20" customHeight="1">
       <c r="A17" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B17" s="1">
-        <v>201</v>
+        <v>41</v>
       </c>
       <c r="C17" s="1">
-        <v>220</v>
+        <v>74</v>
       </c>
       <c r="D17" s="1">
         <v>0</v>
@@ -994,46 +892,46 @@
         <v>0</v>
       </c>
       <c r="G17" s="1">
-        <v>0</v>
+        <v>31</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="I17" s="1">
-        <v>59</v>
+        <v>16</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="20" customHeight="1">
       <c r="H18" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="I18" s="1">
-        <v>64</v>
+        <v>4</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>31</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="20" customHeight="1">
       <c r="H19" s="1" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="I19" s="1">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="20" customHeight="1">
       <c r="H20" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I20" s="1">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>31</v>
@@ -1041,64 +939,106 @@
     </row>
     <row r="21" spans="1:10" ht="20" customHeight="1">
       <c r="H21" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="I21" s="1">
-        <v>24</v>
+        <v>1</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="20" customHeight="1">
       <c r="A22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1">
+        <v>49</v>
+      </c>
+      <c r="C22" s="1">
+        <v>80</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0</v>
+      </c>
+      <c r="E22" s="1">
+        <v>0</v>
+      </c>
+      <c r="F22" s="1">
+        <v>0</v>
+      </c>
+      <c r="G22" s="1">
+        <v>0</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="1">
+        <v>49</v>
+      </c>
+      <c r="J22" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="20" customHeight="1">
+      <c r="A23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23" s="1">
+        <v>32</v>
+      </c>
+      <c r="C23" s="1">
+        <v>149</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0</v>
+      </c>
+      <c r="E23" s="1">
+        <v>0</v>
+      </c>
+      <c r="F23" s="1">
+        <v>0</v>
+      </c>
+      <c r="G23" s="1">
+        <v>0</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I23" s="1">
+        <v>32</v>
+      </c>
+      <c r="J23" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="20" customHeight="1">
+      <c r="A24" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="1">
+        <v>79</v>
+      </c>
+      <c r="C24" s="1">
+        <v>240</v>
+      </c>
+      <c r="D24" s="1">
         <v>24</v>
       </c>
-      <c r="B22" s="1">
-        <v>565</v>
-      </c>
-      <c r="C22" s="1">
-        <v>1050</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0</v>
-      </c>
-      <c r="E22" s="1">
-        <v>0</v>
-      </c>
-      <c r="F22" s="1">
-        <v>0</v>
-      </c>
-      <c r="G22" s="1">
-        <v>871</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I22" s="1">
-        <v>194</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="20" customHeight="1">
-      <c r="H23" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I23" s="1">
-        <v>27</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="20" customHeight="1">
+      <c r="E24" s="1">
+        <v>64</v>
+      </c>
+      <c r="F24" s="1">
+        <v>88</v>
+      </c>
+      <c r="G24" s="1">
+        <v>173</v>
+      </c>
       <c r="H24" s="1" t="s">
-        <v>24</v>
+        <v>13</v>
       </c>
       <c r="I24" s="1">
-        <v>1000</v>
+        <v>51</v>
       </c>
       <c r="J24" s="1" t="s">
         <v>37</v>
@@ -1106,68 +1046,47 @@
     </row>
     <row r="25" spans="1:10" ht="20" customHeight="1">
       <c r="H25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I25" s="1">
+        <v>4</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="20" customHeight="1">
+      <c r="H26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I26" s="1">
         <v>24</v>
       </c>
-      <c r="I25" s="1">
-        <v>200</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="20" customHeight="1">
-      <c r="A26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="1">
-        <v>81</v>
-      </c>
-      <c r="C26" s="1">
-        <v>280</v>
-      </c>
-      <c r="D26" s="1">
-        <v>11</v>
-      </c>
-      <c r="E26" s="1">
-        <v>0</v>
-      </c>
-      <c r="F26" s="1">
-        <v>0</v>
-      </c>
-      <c r="G26" s="1">
-        <v>0</v>
-      </c>
-      <c r="H26" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="I26" s="1">
-        <v>81</v>
-      </c>
       <c r="J26" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="20" customHeight="1">
       <c r="A27" s="1" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B27" s="1">
-        <v>115</v>
+        <v>1</v>
       </c>
       <c r="C27" s="1">
-        <v>329</v>
+        <v>1</v>
       </c>
       <c r="D27" s="1">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="E27" s="1">
-        <v>249</v>
+        <v>0</v>
       </c>
       <c r="F27" s="1">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="G27" s="1">
-        <v>581</v>
+        <v>0</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>21</v>
@@ -1176,50 +1095,461 @@
         <v>1</v>
       </c>
       <c r="J27" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" ht="20" customHeight="1">
+      <c r="A28" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28" s="1">
+        <v>72</v>
+      </c>
+      <c r="C28" s="1">
+        <v>490</v>
+      </c>
+      <c r="D28" s="1">
+        <v>64</v>
+      </c>
+      <c r="E28" s="1">
+        <v>180</v>
+      </c>
+      <c r="F28" s="1">
+        <v>160</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I28" s="1">
+        <v>3</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="20" customHeight="1">
+      <c r="H29" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I29" s="1">
+        <v>66</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" ht="20" customHeight="1">
+      <c r="H30" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="1">
+        <v>3</v>
+      </c>
+      <c r="J30" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="20" customHeight="1">
+      <c r="A31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B31" s="1">
+        <v>5</v>
+      </c>
+      <c r="C31" s="1">
+        <v>428</v>
+      </c>
+      <c r="D31" s="1">
+        <v>42</v>
+      </c>
+      <c r="E31" s="1">
+        <v>47</v>
+      </c>
+      <c r="F31" s="1">
+        <v>0</v>
+      </c>
+      <c r="G31" s="1">
+        <v>124</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I31" s="1">
+        <v>5</v>
+      </c>
+      <c r="J31" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="20" customHeight="1">
-      <c r="H28" s="1" t="s">
+    <row r="32" spans="1:10" ht="20" customHeight="1">
+      <c r="A32" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32" s="1">
+        <v>19</v>
+      </c>
+      <c r="C32" s="1">
+        <v>125</v>
+      </c>
+      <c r="D32" s="1">
+        <v>0</v>
+      </c>
+      <c r="E32" s="1">
+        <v>0</v>
+      </c>
+      <c r="F32" s="1">
+        <v>10</v>
+      </c>
+      <c r="G32" s="1">
+        <v>35</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I32" s="1">
+        <v>19</v>
+      </c>
+      <c r="J32" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="20" customHeight="1">
+      <c r="A33" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="1">
+        <v>201</v>
+      </c>
+      <c r="C33" s="1">
+        <v>220</v>
+      </c>
+      <c r="D33" s="1">
+        <v>0</v>
+      </c>
+      <c r="E33" s="1">
+        <v>0</v>
+      </c>
+      <c r="F33" s="1">
+        <v>0</v>
+      </c>
+      <c r="G33" s="1">
+        <v>0</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I33" s="1">
+        <v>61</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="20" customHeight="1">
+      <c r="H34" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="I28" s="1">
-        <v>114</v>
-      </c>
-      <c r="J28" s="1" t="s">
+      <c r="I34" s="1">
+        <v>98</v>
+      </c>
+      <c r="J34" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="20" customHeight="1">
+      <c r="H35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I35" s="1">
+        <v>42</v>
+      </c>
+      <c r="J35" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" ht="20" customHeight="1">
+      <c r="A36" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B36" s="1">
+        <v>565</v>
+      </c>
+      <c r="C36" s="1">
+        <v>3050</v>
+      </c>
+      <c r="D36" s="1">
+        <v>0</v>
+      </c>
+      <c r="E36" s="1">
+        <v>0</v>
+      </c>
+      <c r="F36" s="1">
+        <v>0</v>
+      </c>
+      <c r="G36" s="1">
+        <v>871</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I36" s="1">
+        <v>53</v>
+      </c>
+      <c r="J36" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" ht="20" customHeight="1">
+      <c r="H37" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="I37" s="1">
+        <v>14</v>
+      </c>
+      <c r="J37" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="20" customHeight="1">
+      <c r="H38" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="I38" s="1">
+        <v>19</v>
+      </c>
+      <c r="J38" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" ht="20" customHeight="1">
+      <c r="H39" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I39" s="1">
+        <v>249</v>
+      </c>
+      <c r="J39" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="20" customHeight="1">
-      <c r="A29" s="1" t="s">
+    <row r="40" spans="1:10" ht="20" customHeight="1">
+      <c r="H40" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I40" s="1">
+        <v>10</v>
+      </c>
+      <c r="J40" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="20" customHeight="1">
+      <c r="H41" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I41" s="1">
+        <v>21</v>
+      </c>
+      <c r="J41" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" ht="20" customHeight="1">
+      <c r="H42" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I42" s="1">
+        <v>64</v>
+      </c>
+      <c r="J42" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="20" customHeight="1">
+      <c r="H43" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="I43" s="1">
+        <v>24</v>
+      </c>
+      <c r="J43" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" ht="20" customHeight="1">
+      <c r="H44" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" s="1">
+        <v>11</v>
+      </c>
+      <c r="J44" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" ht="20" customHeight="1">
+      <c r="H45" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I45" s="1">
+        <v>1</v>
+      </c>
+      <c r="J45" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" ht="20" customHeight="1">
+      <c r="H46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I46" s="1">
+        <v>4</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="20" customHeight="1">
+      <c r="H47" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I47" s="1">
+        <v>95</v>
+      </c>
+      <c r="J47" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="20" customHeight="1">
+      <c r="A48" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="1">
+      <c r="B48" s="1">
+        <v>81</v>
+      </c>
+      <c r="C48" s="1">
+        <v>280</v>
+      </c>
+      <c r="D48" s="1">
+        <v>11</v>
+      </c>
+      <c r="E48" s="1">
+        <v>0</v>
+      </c>
+      <c r="F48" s="1">
+        <v>0</v>
+      </c>
+      <c r="G48" s="1">
+        <v>0</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I48" s="1">
+        <v>81</v>
+      </c>
+      <c r="J48" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="20" customHeight="1">
+      <c r="A49" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B49" s="1">
+        <v>115</v>
+      </c>
+      <c r="C49" s="1">
+        <v>329</v>
+      </c>
+      <c r="D49" s="1">
+        <v>95</v>
+      </c>
+      <c r="E49" s="1">
+        <v>249</v>
+      </c>
+      <c r="F49" s="1">
+        <v>69</v>
+      </c>
+      <c r="G49" s="1">
+        <v>581</v>
+      </c>
+      <c r="H49" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I49" s="1">
+        <v>2</v>
+      </c>
+      <c r="J49" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="20" customHeight="1">
+      <c r="H50" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I50" s="1">
+        <v>12</v>
+      </c>
+      <c r="J50" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="20" customHeight="1">
+      <c r="H51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I51" s="1">
+        <v>101</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="20" customHeight="1">
+      <c r="A52" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B52" s="1">
         <v>36</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C52" s="1">
         <v>119</v>
       </c>
-      <c r="D29" s="1">
-        <v>0</v>
-      </c>
-      <c r="E29" s="1">
-        <v>0</v>
-      </c>
-      <c r="F29" s="1">
+      <c r="D52" s="1">
+        <v>0</v>
+      </c>
+      <c r="E52" s="1">
+        <v>0</v>
+      </c>
+      <c r="F52" s="1">
         <v>1</v>
       </c>
-      <c r="G29" s="1">
+      <c r="G52" s="1">
         <v>19</v>
       </c>
-      <c r="H29" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="I29" s="1">
-        <v>36</v>
-      </c>
-      <c r="J29" s="1" t="s">
-        <v>29</v>
+      <c r="H52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="I52" s="1">
+        <v>20</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="20" customHeight="1">
+      <c r="H53" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I53" s="1">
+        <v>16</v>
+      </c>
+      <c r="J53" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>